<commit_message>
Data tables for character avatar reactions / animations
</commit_message>
<xml_diff>
--- a/Misc/MM8_CHAR_SOUNDS_EXPRESSIONS.xlsx
+++ b/Misc/MM8_CHAR_SOUNDS_EXPRESSIONS.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjasi\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z003jymv\Github\OpenMM8\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74F1E2B-950B-407A-BB30-D2BB900E57C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BC8ACF-41C1-4480-93F0-92E5BF7BA090}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{830A5CC2-0CC8-42D9-BECB-D27FEFA601A0}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{830A5CC2-0CC8-42D9-BECB-D27FEFA601A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="259">
   <si>
     <t>subvariant</t>
   </si>
@@ -264,9 +270,6 @@
     <t>Last Man Standing</t>
   </si>
   <si>
-    <t>End Of Hard Fight</t>
-  </si>
-  <si>
     <t>Enter Dungeon</t>
   </si>
   <si>
@@ -468,12 +471,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Action_1</t>
-  </si>
-  <si>
-    <t>Action_2</t>
-  </si>
-  <si>
     <t>PlaceIsClosed</t>
   </si>
   <si>
@@ -505,6 +502,312 @@
   </si>
   <si>
     <t>CannotRestHere</t>
+  </si>
+  <si>
+    <t>SkillUp</t>
+  </si>
+  <si>
+    <t>NoInventoryRoom</t>
+  </si>
+  <si>
+    <t>PotionMixFail</t>
+  </si>
+  <si>
+    <t>PotionMixOk</t>
+  </si>
+  <si>
+    <t>LockedNeedAKey</t>
+  </si>
+  <si>
+    <t>CannotLearnThat</t>
+  </si>
+  <si>
+    <t>LearnOk</t>
+  </si>
+  <si>
+    <t>GoodEvening</t>
+  </si>
+  <si>
+    <t>DamagedOww</t>
+  </si>
+  <si>
+    <t>Weakened</t>
+  </si>
+  <si>
+    <t>Feared</t>
+  </si>
+  <si>
+    <t>Poisoned</t>
+  </si>
+  <si>
+    <t>Diseased</t>
+  </si>
+  <si>
+    <t>Cursed</t>
+  </si>
+  <si>
+    <t>Unconcious</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Petrified</t>
+  </si>
+  <si>
+    <t>Eradicated</t>
+  </si>
+  <si>
+    <t>SmileGood</t>
+  </si>
+  <si>
+    <t>ReadScroll</t>
+  </si>
+  <si>
+    <t>NotEnoughGold</t>
+  </si>
+  <si>
+    <t>CannotEquipItem</t>
+  </si>
+  <si>
+    <t>ItemBrokenOrStolen</t>
+  </si>
+  <si>
+    <t>GotManaDrained</t>
+  </si>
+  <si>
+    <t>Aged</t>
+  </si>
+  <si>
+    <t>CastedSpell</t>
+  </si>
+  <si>
+    <t>maybe_receive_damage_anim</t>
+  </si>
+  <si>
+    <t>frames: duration = usually 8 or 16</t>
+  </si>
+  <si>
+    <t>It is multiplied by 8</t>
+  </si>
+  <si>
+    <t>8 * 8 = 64 = 0.5s</t>
+  </si>
+  <si>
+    <t>8 * 16 = 1s</t>
+  </si>
+  <si>
+    <t>"128" = 1 seconds in original engine</t>
+  </si>
+  <si>
+    <t>unk - anim only</t>
+  </si>
+  <si>
+    <t>EnterDungeon</t>
+  </si>
+  <si>
+    <t>End Of Hard Fight (Leave dungeon in combat)</t>
+  </si>
+  <si>
+    <t>LeaveDungeonInCombat</t>
+  </si>
+  <si>
+    <t>ModeratelyInjured</t>
+  </si>
+  <si>
+    <t>FailedToEnchantItem</t>
+  </si>
+  <si>
+    <t>ShotBow</t>
+  </si>
+  <si>
+    <t>BigMonsterKilled</t>
+  </si>
+  <si>
+    <t>SmallMonsterKilled (Player.cpp:7085)</t>
+  </si>
+  <si>
+    <t>MonsterKilledGeneric</t>
+  </si>
+  <si>
+    <t>MissedAttack</t>
+  </si>
+  <si>
+    <t>YellMove</t>
+  </si>
+  <si>
+    <t>FallingScrem</t>
+  </si>
+  <si>
+    <t>ThatWasRude</t>
+  </si>
+  <si>
+    <t>GoodDay_2</t>
+  </si>
+  <si>
+    <t>GoodDay_1</t>
+  </si>
+  <si>
+    <t>PickMe</t>
+  </si>
+  <si>
+    <t>CannotIdentifyMonster</t>
+  </si>
+  <si>
+    <t>IdentifyWeakMonster</t>
+  </si>
+  <si>
+    <t>IdentifyStrongMonster</t>
+  </si>
+  <si>
+    <t>LastManStanding</t>
+  </si>
+  <si>
+    <t>FatallyInjured</t>
+  </si>
+  <si>
+    <t>Unknown_110</t>
+  </si>
+  <si>
+    <t>Unknown_53</t>
+  </si>
+  <si>
+    <t>Unknown_54</t>
+  </si>
+  <si>
+    <t>Unknown_55</t>
+  </si>
+  <si>
+    <t>Unknown_56</t>
+  </si>
+  <si>
+    <t>Unknown_57</t>
+  </si>
+  <si>
+    <t>Unknown_58</t>
+  </si>
+  <si>
+    <t>Unknown_59</t>
+  </si>
+  <si>
+    <t>Unknown_62</t>
+  </si>
+  <si>
+    <t>Unknown_68</t>
+  </si>
+  <si>
+    <t>Unknown_69</t>
+  </si>
+  <si>
+    <t>Unknown_70</t>
+  </si>
+  <si>
+    <t>Unknown_88</t>
+  </si>
+  <si>
+    <t>Unknown_89</t>
+  </si>
+  <si>
+    <t>Unknown_90</t>
+  </si>
+  <si>
+    <t>Unknown_94</t>
+  </si>
+  <si>
+    <t>Unknown_95</t>
+  </si>
+  <si>
+    <t>Unknown_97</t>
+  </si>
+  <si>
+    <t>Unknown_98</t>
+  </si>
+  <si>
+    <t>Unknown_100</t>
+  </si>
+  <si>
+    <t>Unknown_101</t>
+  </si>
+  <si>
+    <t>FoundGold</t>
+  </si>
+  <si>
+    <t>HiredNpc</t>
+  </si>
+  <si>
+    <t>LookUp</t>
+  </si>
+  <si>
+    <t>LookDown</t>
+  </si>
+  <si>
+    <t>HaveMoreFoodThanYou</t>
+  </si>
+  <si>
+    <t>TravelByCarriage</t>
+  </si>
+  <si>
+    <t>TravelByBoat</t>
+  </si>
+  <si>
+    <t>ShopIdentifiedItem</t>
+  </si>
+  <si>
+    <t>ShopRepairedItem</t>
+  </si>
+  <si>
+    <t>ShopBoughtItem</t>
+  </si>
+  <si>
+    <t>ShopItemAlreadyRepairedOrIdentified</t>
+  </si>
+  <si>
+    <t>ShopSoldItem</t>
+  </si>
+  <si>
+    <t>ShopLearnedSkill</t>
+  </si>
+  <si>
+    <t>ShopWrongActionOnItem</t>
+  </si>
+  <si>
+    <t>ShopStoredGoldInBank</t>
+  </si>
+  <si>
+    <t>ShopHealedInTemple</t>
+  </si>
+  <si>
+    <t>ShopDonatedInTemple</t>
+  </si>
+  <si>
+    <t>JoinedGuild_1</t>
+  </si>
+  <si>
+    <t>JoinedGuild_2</t>
+  </si>
+  <si>
+    <t>TrainedToNextLevel</t>
+  </si>
+  <si>
+    <t>ReceivedTemporaryStatBonus</t>
+  </si>
+  <si>
+    <t>ReceivedPermanentStatBonus</t>
+  </si>
+  <si>
+    <t>QuestDone</t>
+  </si>
+  <si>
+    <t>ReceivedAward</t>
+  </si>
+  <si>
+    <t>BecameZombie</t>
+  </si>
+  <si>
+    <t>WokeUp</t>
+  </si>
+  <si>
+    <t>Unknown_19</t>
   </si>
 </sst>
 </file>
@@ -723,11 +1026,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -752,6 +1052,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1073,24 +1379,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62B4B90-75E9-4908-936C-C0FD62A1FCFB}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1098,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1114,1877 +1420,2139 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
         <f>B2+2*(B1+50*B3)+4998</f>
         <v>5000</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="J10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="J10" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <f>$B$2+2*(B11+50*$B$3)+4998</f>
         <v>5000</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>47</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>147</v>
+      <c r="H11" s="16" t="s">
+        <v>197</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
         <f t="shared" ref="A12:A57" si="0">$B$2+2*(B12+50*$B$3)+4998</f>
         <v>5002</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="7">
         <v>25</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>148</v>
+      <c r="H12" s="16" t="s">
+        <v>196</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>5004</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>3</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="E13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="7">
         <v>41.42</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>149</v>
+      <c r="H13" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="I13">
         <v>3</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>5006</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>4</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="8"/>
+      <c r="E14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="7"/>
       <c r="G14">
         <v>4</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>150</v>
+      <c r="H14" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="I14">
         <v>4</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>5008</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>5</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="G15">
         <v>5</v>
       </c>
-      <c r="H15" s="17" t="s">
-        <v>151</v>
+      <c r="H15" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="I15">
         <v>5</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>5010</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>6</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="E16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="7">
         <v>47</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
-      <c r="H16" s="17" t="s">
-        <v>152</v>
+      <c r="H16" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="I16">
         <v>6</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>5012</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>7</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="E17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="7">
         <v>43.48</v>
       </c>
       <c r="G17">
         <v>7</v>
       </c>
-      <c r="H17" s="17" t="s">
-        <v>153</v>
+      <c r="H17" s="16" t="s">
+        <v>150</v>
       </c>
       <c r="I17">
         <v>7</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="16">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>5014</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>8</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="7">
         <v>38</v>
       </c>
       <c r="G18">
         <v>8</v>
       </c>
-      <c r="H18" s="17" t="s">
-        <v>154</v>
+      <c r="H18" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="I18">
         <v>8</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>5016</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>9</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="E19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="7">
         <v>39</v>
       </c>
       <c r="G19">
         <v>9</v>
       </c>
-      <c r="H19" s="17" t="s">
-        <v>155</v>
+      <c r="H19" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="I19">
         <v>9</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="16">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>5018</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>10</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="D20" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="7">
         <v>45</v>
       </c>
       <c r="G20">
         <v>10</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>156</v>
+      <c r="H20" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="I20">
         <v>10</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="16">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>5020</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>11</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="D21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="7">
         <v>47</v>
       </c>
       <c r="G21">
         <v>11</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>157</v>
+      <c r="H21" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="I21">
         <v>11</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="16">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>5022</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>12</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="7">
         <v>43.48</v>
       </c>
       <c r="G22">
         <v>12</v>
       </c>
-      <c r="H22" s="17" t="s">
-        <v>158</v>
+      <c r="H22" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="I22">
         <v>12</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="16">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>5024</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>13</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="8">
+      <c r="E23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="7">
         <v>37.380000000000003</v>
       </c>
       <c r="G23">
         <v>13</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>159</v>
+      <c r="H23" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="I23">
         <v>13</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="16">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>5026</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>14</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="8">
+      <c r="E24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="7">
         <v>48</v>
       </c>
       <c r="G24">
         <v>14</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="16" t="s">
+        <v>157</v>
+      </c>
       <c r="I24">
         <v>14</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="16">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>5028</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>15</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="G25">
         <v>15</v>
       </c>
-      <c r="H25" s="17"/>
+      <c r="H25" s="16" t="s">
+        <v>158</v>
+      </c>
       <c r="I25">
         <v>15</v>
       </c>
-      <c r="J25" s="17">
+      <c r="J25" s="16">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>5030</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>16</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="8">
+      <c r="E26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="7">
         <v>46</v>
       </c>
       <c r="G26">
         <v>16</v>
       </c>
-      <c r="H26" s="17"/>
+      <c r="H26" s="16" t="s">
+        <v>160</v>
+      </c>
       <c r="I26">
         <v>16</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="16">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>5032</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>17</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F27" s="8"/>
+      <c r="D27" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="7"/>
       <c r="G27">
         <v>17</v>
       </c>
-      <c r="H27" s="17"/>
+      <c r="H27" s="16" t="s">
+        <v>159</v>
+      </c>
       <c r="I27">
         <v>17</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J27" s="16">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>5034</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>18</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F28" s="8">
+      <c r="E28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="7">
         <v>6</v>
       </c>
       <c r="G28">
         <v>18</v>
       </c>
-      <c r="H28" s="17"/>
+      <c r="H28" s="16" t="s">
+        <v>161</v>
+      </c>
       <c r="I28">
         <v>18</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="16">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>5036</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>19</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="8">
+      <c r="E29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="7">
         <v>7</v>
       </c>
       <c r="G29">
         <v>19</v>
       </c>
-      <c r="H29" s="17"/>
+      <c r="H29" s="16" t="s">
+        <v>258</v>
+      </c>
       <c r="I29">
         <v>19</v>
       </c>
-      <c r="J29" s="17">
+      <c r="J29" s="16">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>5038</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>20</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="G30">
         <v>20</v>
       </c>
-      <c r="H30" s="17"/>
+      <c r="H30" s="16" t="s">
+        <v>162</v>
+      </c>
       <c r="I30">
         <v>20</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30" s="16">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>21</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F31" s="8">
+      <c r="E31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="7">
         <v>2</v>
       </c>
       <c r="G31">
         <v>21</v>
       </c>
-      <c r="H31" s="17"/>
+      <c r="H31" s="16" t="s">
+        <v>163</v>
+      </c>
       <c r="I31">
         <v>21</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="16">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>5042</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>22</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="G32">
         <v>22</v>
       </c>
-      <c r="H32" s="17"/>
+      <c r="H32" s="16" t="s">
+        <v>204</v>
+      </c>
       <c r="I32">
         <v>22</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J32" s="16">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>5044</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>23</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="E33" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" s="7">
         <v>25</v>
       </c>
       <c r="G33">
         <v>23</v>
       </c>
-      <c r="H33" s="17"/>
+      <c r="H33" s="16" t="s">
+        <v>164</v>
+      </c>
       <c r="I33">
         <v>23</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J33" s="16">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>5046</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>24</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="8">
+      <c r="E34" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="7">
         <v>25</v>
       </c>
       <c r="G34">
         <v>24</v>
       </c>
-      <c r="H34" s="17"/>
+      <c r="H34" s="16" t="s">
+        <v>165</v>
+      </c>
       <c r="I34">
         <v>24</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="16">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>5048</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>25</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F35" s="8">
+      <c r="E35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="7">
         <v>25</v>
       </c>
       <c r="G35">
         <v>25</v>
       </c>
-      <c r="H35" s="17"/>
+      <c r="H35" s="16" t="s">
+        <v>166</v>
+      </c>
       <c r="I35">
         <v>25</v>
       </c>
-      <c r="J35" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="J35" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>5050</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>26</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F36" s="8">
+      <c r="E36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="7">
         <v>38.47</v>
       </c>
       <c r="G36">
         <v>26</v>
       </c>
-      <c r="H36" s="17"/>
+      <c r="H36" s="16" t="s">
+        <v>167</v>
+      </c>
       <c r="I36">
         <v>26</v>
       </c>
-      <c r="J36" s="17"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>5052</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>27</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F37" s="8">
+      <c r="E37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F37" s="7">
         <v>42.42</v>
       </c>
       <c r="G37">
         <v>27</v>
       </c>
-      <c r="H37" s="17"/>
+      <c r="H37" s="16" t="s">
+        <v>168</v>
+      </c>
       <c r="I37">
         <v>27</v>
       </c>
-      <c r="J37" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+      <c r="J37" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>5054</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>28</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="8">
+      <c r="E38" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" s="7">
         <v>25</v>
       </c>
       <c r="G38">
         <v>28</v>
       </c>
-      <c r="H38" s="17"/>
+      <c r="H38" s="16" t="s">
+        <v>169</v>
+      </c>
       <c r="I38">
         <v>28</v>
       </c>
-      <c r="J38" s="17"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>5056</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>29</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F39" s="8">
+      <c r="E39" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="7">
         <v>27</v>
       </c>
       <c r="G39">
         <v>29</v>
       </c>
-      <c r="H39" s="17"/>
+      <c r="H39" s="16" t="s">
+        <v>64</v>
+      </c>
       <c r="I39">
         <v>29</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="16">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>5058</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>30</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" s="8">
+      <c r="E40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" s="7">
         <v>25</v>
       </c>
       <c r="G40">
         <v>30</v>
       </c>
-      <c r="H40" s="17"/>
+      <c r="H40" s="16" t="s">
+        <v>170</v>
+      </c>
       <c r="I40">
         <v>30</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="16">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>5060</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>31</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F41" s="8">
+      <c r="E41" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F41" s="7">
         <v>25</v>
       </c>
       <c r="G41">
         <v>31</v>
       </c>
-      <c r="H41" s="17"/>
+      <c r="H41" s="16" t="s">
+        <v>63</v>
+      </c>
       <c r="I41">
         <v>31</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J41" s="16">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
         <f t="shared" si="0"/>
         <v>5062</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>32</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F42" s="8" t="s">
+      <c r="E42" s="2" t="s">
         <v>126</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="G42">
         <v>32</v>
       </c>
+      <c r="H42" s="16" t="s">
+        <v>171</v>
+      </c>
       <c r="I42">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
         <f t="shared" si="0"/>
         <v>5064</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>33</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" s="8" t="s">
+      <c r="E43" s="2" t="s">
         <v>126</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="G43">
         <v>33</v>
       </c>
-      <c r="H43" s="17"/>
+      <c r="H43" s="16" t="s">
+        <v>172</v>
+      </c>
       <c r="I43">
         <v>33</v>
       </c>
-      <c r="J43" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+      <c r="J43" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
         <f t="shared" si="0"/>
         <v>5066</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>34</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F44" s="8">
+      <c r="E44" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="7">
         <v>53</v>
       </c>
       <c r="G44">
         <v>34</v>
       </c>
-      <c r="H44" s="17"/>
+      <c r="H44" s="16" t="s">
+        <v>173</v>
+      </c>
       <c r="I44">
         <v>34</v>
       </c>
-      <c r="J44" s="17">
+      <c r="J44" s="16">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
         <f t="shared" si="0"/>
         <v>5068</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>35</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="8"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="7"/>
       <c r="G45">
         <v>35</v>
       </c>
-      <c r="H45" s="17"/>
+      <c r="H45" s="16" t="s">
+        <v>174</v>
+      </c>
       <c r="I45">
         <v>35</v>
       </c>
-      <c r="J45" s="17">
+      <c r="J45" s="16">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
         <f t="shared" si="0"/>
         <v>5070</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>36</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="8"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="7"/>
       <c r="G46">
         <v>36</v>
       </c>
-      <c r="H46" s="17"/>
+      <c r="H46" s="16" t="s">
+        <v>175</v>
+      </c>
       <c r="I46">
         <v>36</v>
       </c>
-      <c r="J46" s="17">
+      <c r="J46" s="16">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
         <f t="shared" si="0"/>
         <v>5072</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>37</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F47" s="8">
+      <c r="E47" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="7">
         <v>47.53</v>
       </c>
       <c r="G47">
         <v>37</v>
       </c>
-      <c r="H47" s="17"/>
+      <c r="H47" s="16" t="s">
+        <v>176</v>
+      </c>
       <c r="I47">
         <v>37</v>
       </c>
-      <c r="J47" s="17">
+      <c r="J47" s="16">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
         <f t="shared" si="0"/>
         <v>5074</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>38</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="G48">
         <v>38</v>
       </c>
-      <c r="H48" s="17"/>
+      <c r="H48" s="16" t="s">
+        <v>177</v>
+      </c>
       <c r="I48">
         <v>38</v>
       </c>
-      <c r="J48" s="17">
+      <c r="J48" s="16">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
         <f t="shared" si="0"/>
         <v>5076</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>39</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="E49" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" s="7">
         <v>48</v>
       </c>
       <c r="G49">
         <v>39</v>
       </c>
-      <c r="H49" s="17"/>
+      <c r="H49" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="I49">
         <v>39</v>
       </c>
-      <c r="J49" s="17">
+      <c r="J49" s="16">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
         <f t="shared" si="0"/>
         <v>5078</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>40</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F50" s="8">
+        <v>191</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50" s="7">
         <v>21</v>
       </c>
       <c r="G50">
         <v>40</v>
       </c>
-      <c r="H50" s="17"/>
+      <c r="H50" s="16" t="s">
+        <v>179</v>
+      </c>
       <c r="I50">
         <v>40</v>
       </c>
-      <c r="J50" s="17">
+      <c r="J50" s="16">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
         <f t="shared" si="0"/>
         <v>5080</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>41</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F51" s="8">
+      <c r="D51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F51" s="7">
         <v>21</v>
       </c>
       <c r="G51">
         <v>41</v>
       </c>
-      <c r="H51" s="17"/>
+      <c r="H51" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="I51">
         <v>41</v>
       </c>
-      <c r="J51" s="17">
+      <c r="J51" s="16">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
         <f t="shared" si="0"/>
         <v>5082</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>42</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="8"/>
+      <c r="D52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="7"/>
       <c r="G52">
         <v>42</v>
       </c>
-      <c r="H52" s="17"/>
+      <c r="H52" s="16" t="s">
+        <v>181</v>
+      </c>
       <c r="I52">
         <v>42</v>
       </c>
-      <c r="J52" s="17">
+      <c r="J52" s="16">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
         <f t="shared" si="0"/>
         <v>5084</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>43</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="8"/>
+      <c r="D53" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="7"/>
       <c r="G53">
         <v>43</v>
       </c>
-      <c r="H53" s="17"/>
+      <c r="H53" s="16" t="s">
+        <v>194</v>
+      </c>
       <c r="I53">
         <v>43</v>
       </c>
-      <c r="J53" s="17">
+      <c r="J53" s="16">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
         <f t="shared" si="0"/>
         <v>5086</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>44</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="D54" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F54" s="8">
+      <c r="E54" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" s="7">
         <v>39.479999999999997</v>
       </c>
       <c r="G54">
         <v>44</v>
       </c>
-      <c r="H54" s="17"/>
+      <c r="H54" s="16" t="s">
+        <v>183</v>
+      </c>
       <c r="I54">
         <v>44</v>
       </c>
-      <c r="J54" s="17">
+      <c r="J54" s="16">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="6">
         <f t="shared" si="0"/>
         <v>5088</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="2">
         <v>45</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="8"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="7"/>
       <c r="G55">
         <v>45</v>
       </c>
-      <c r="H55" s="17"/>
+      <c r="H55" s="16" t="s">
+        <v>189</v>
+      </c>
       <c r="I55">
         <v>45</v>
       </c>
-      <c r="J55" s="17">
+      <c r="J55" s="16">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
         <f t="shared" si="0"/>
         <v>5090</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <v>46</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="8"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="7"/>
       <c r="G56">
         <v>46</v>
       </c>
-      <c r="H56" s="17"/>
+      <c r="H56" s="16" t="s">
+        <v>190</v>
+      </c>
       <c r="I56">
         <v>46</v>
       </c>
-      <c r="J56" s="17">
+      <c r="J56" s="16">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9">
+    <row r="57" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="8">
         <f t="shared" si="0"/>
         <v>5092</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="9">
         <v>47</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D57" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F57" s="11">
+      <c r="D57" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" s="10">
         <v>46</v>
       </c>
       <c r="G57">
         <v>47</v>
       </c>
-      <c r="H57" s="17"/>
+      <c r="H57" s="16" t="s">
+        <v>192</v>
+      </c>
       <c r="I57">
         <v>47</v>
       </c>
-      <c r="J57" s="17">
+      <c r="J57" s="16">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F58" s="2"/>
+    <row r="58" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="1"/>
       <c r="G58">
         <v>48</v>
       </c>
-      <c r="H58" s="17"/>
+      <c r="H58" s="16" t="s">
+        <v>193</v>
+      </c>
       <c r="I58">
         <v>48</v>
       </c>
-      <c r="J58" s="17">
+      <c r="J58" s="16">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F59" s="2"/>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F59" s="1"/>
       <c r="G59">
         <v>49</v>
       </c>
-      <c r="H59" s="17"/>
+      <c r="H59" s="16" t="s">
+        <v>182</v>
+      </c>
       <c r="I59">
         <v>49</v>
       </c>
-      <c r="J59" s="17">
+      <c r="J59" s="16">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G60">
         <v>50</v>
       </c>
-      <c r="H60" s="17"/>
+      <c r="H60" s="16" t="s">
+        <v>195</v>
+      </c>
       <c r="I60">
         <v>50</v>
       </c>
-      <c r="J60" s="17">
+      <c r="J60" s="16">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G61">
         <v>51</v>
       </c>
-      <c r="H61" s="17"/>
+      <c r="H61" s="16" t="s">
+        <v>198</v>
+      </c>
       <c r="I61">
         <v>51</v>
       </c>
-      <c r="J61" s="17">
+      <c r="J61" s="16">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>184</v>
+      </c>
       <c r="G62">
         <v>52</v>
       </c>
-      <c r="H62" s="17"/>
+      <c r="H62" s="16" t="s">
+        <v>199</v>
+      </c>
       <c r="I62">
         <v>52</v>
       </c>
-      <c r="J62" s="17">
+      <c r="J62" s="16">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>185</v>
+      </c>
       <c r="G63">
         <v>53</v>
       </c>
-      <c r="H63" s="17"/>
+      <c r="H63" s="16" t="s">
+        <v>212</v>
+      </c>
       <c r="I63">
         <v>53</v>
       </c>
-      <c r="J63" s="17">
+      <c r="J63" s="16">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>186</v>
+      </c>
       <c r="G64">
         <v>54</v>
       </c>
-      <c r="H64" s="17"/>
+      <c r="H64" s="16" t="s">
+        <v>213</v>
+      </c>
       <c r="I64">
         <v>54</v>
       </c>
-      <c r="J64" s="17">
+      <c r="J64" s="16">
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>187</v>
+      </c>
       <c r="G65">
         <v>55</v>
       </c>
-      <c r="H65" s="17"/>
+      <c r="H65" s="16" t="s">
+        <v>214</v>
+      </c>
       <c r="I65">
         <v>55</v>
       </c>
-      <c r="J65" s="17">
+      <c r="J65" s="16">
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>188</v>
+      </c>
       <c r="G66">
         <v>56</v>
       </c>
-      <c r="H66" s="17"/>
+      <c r="H66" s="16" t="s">
+        <v>215</v>
+      </c>
       <c r="I66">
         <v>56</v>
       </c>
-      <c r="J66" s="17">
+      <c r="J66" s="16">
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G67">
         <v>57</v>
       </c>
-      <c r="H67" s="17"/>
+      <c r="H67" s="16" t="s">
+        <v>216</v>
+      </c>
       <c r="I67">
         <v>57</v>
       </c>
-      <c r="J67" s="17">
+      <c r="J67" s="16">
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G68">
         <v>58</v>
       </c>
-      <c r="H68" s="17"/>
+      <c r="H68" s="16" t="s">
+        <v>217</v>
+      </c>
       <c r="I68">
         <v>58</v>
       </c>
-      <c r="J68" s="17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="69" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="J68" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G69">
         <v>59</v>
       </c>
-    </row>
-    <row r="70" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H69" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="70" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G70">
         <v>60</v>
       </c>
-    </row>
-    <row r="71" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H70" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="71" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G71">
         <v>61</v>
       </c>
-    </row>
-    <row r="72" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H71" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="72" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G72">
         <v>62</v>
       </c>
-    </row>
-    <row r="73" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H72" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="73" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G73">
         <v>63</v>
       </c>
-    </row>
-    <row r="74" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H73" s="16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="74" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G74">
         <v>64</v>
       </c>
-    </row>
-    <row r="75" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H74" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="75" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G75">
         <v>65</v>
       </c>
-    </row>
-    <row r="76" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H75" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G76">
         <v>66</v>
       </c>
-    </row>
-    <row r="77" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H76" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="77" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G77">
         <v>67</v>
       </c>
-    </row>
-    <row r="78" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H77" s="16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="78" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G78">
         <v>68</v>
       </c>
-    </row>
-    <row r="79" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H78" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="79" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G79">
         <v>69</v>
       </c>
-    </row>
-    <row r="80" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H79" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="80" spans="4:10" x14ac:dyDescent="0.3">
       <c r="G80">
         <v>70</v>
       </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G81">
         <v>71</v>
       </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G82">
         <v>72</v>
       </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G83">
         <v>73</v>
       </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G84">
         <v>74</v>
       </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G85">
         <v>75</v>
       </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G86">
         <v>76</v>
       </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G87">
         <v>77</v>
       </c>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G88">
         <v>78</v>
       </c>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G89">
         <v>79</v>
       </c>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="90" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G90">
         <v>80</v>
       </c>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="91" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G91">
         <v>81</v>
       </c>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="92" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G92">
         <v>82</v>
       </c>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="93" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G93">
         <v>83</v>
       </c>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="94" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G94">
         <v>84</v>
       </c>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="95" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G95">
         <v>85</v>
       </c>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="96" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G96">
         <v>86</v>
       </c>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="97" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G97">
         <v>87</v>
       </c>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="98" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G98">
         <v>88</v>
       </c>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="99" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G99">
         <v>89</v>
       </c>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G100">
         <v>90</v>
       </c>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G101">
         <v>91</v>
       </c>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="102" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G102">
         <v>92</v>
       </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="103" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G103">
         <v>93</v>
       </c>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H103" s="16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="104" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G104">
         <v>94</v>
       </c>
-    </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H104" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="105" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G105">
         <v>95</v>
       </c>
-    </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H105" s="16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="106" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G106">
         <v>96</v>
       </c>
-    </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="107" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G107">
         <v>97</v>
       </c>
-    </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G108">
         <v>98</v>
       </c>
-    </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="109" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G109">
         <v>99</v>
       </c>
-    </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="110" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G110">
         <v>100</v>
       </c>
-    </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="111" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G111">
         <v>101</v>
       </c>
-    </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="16" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="112" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G112">
         <v>102</v>
       </c>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H112" s="16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="113" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G113">
         <v>103</v>
       </c>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H113" s="16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="114" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G114">
         <v>104</v>
       </c>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H114" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="115" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G115">
         <v>105</v>
       </c>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H115" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="116" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G116">
         <v>106</v>
       </c>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H116" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="117" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G117">
         <v>107</v>
       </c>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H117" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="118" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G118">
         <v>108</v>
       </c>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H118" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G119">
         <v>109</v>
       </c>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H119" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="120" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G120">
         <v>110</v>
+      </c>
+      <c r="H120" s="16" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>